<commit_message>
CIPW-95% albite to plagioclase
</commit_message>
<xml_diff>
--- a/_CIPW/CIPW/1_normalized_QAPF_count.xlsx
+++ b/_CIPW/CIPW/1_normalized_QAPF_count.xlsx
@@ -380,68 +380,68 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3783</v>
+        <v>3058</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>quartz monzonite</t>
+          <t>granodiorite</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>549</v>
+        <v>908</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>syeno granite</t>
+          <t>quartz monzodiorite
+quartz monzogabbro</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>142</v>
+        <v>394</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>granodiorite</t>
+          <t>quartz monzonite</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>92</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>quartz syenite</t>
+          <t>monzodiorite monzogabbro</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>monzonite</t>
+          <t>syeno granite</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>quartz monzodiorite
-quartz monzogabbro</t>
+          <t>tonalite</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9">
@@ -457,31 +457,33 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>syenite</t>
+          <t>quartz diorite
+quartz gabbro
+quartz anorthosite</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>tonalite</t>
+          <t>monzonite</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>monzodiorite monzogabbro</t>
+          <t>diorite gabbro anorthosite</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
optimizing variogram parameters area1 + qapf classification wtihout P2O5
- Range is quite low, but resulted in best test-values
-Did the CIPW classification for all the datapoints without the P2O5 column to see if there are any differences with previous one (because all the qapf classifications of the areas will also not have the P2O5 column). Very comparable, only small amount of differences. 
- did it only for the normalized values for the qapf. The nonnormalized and the case with the wrong assessment of albite were not altereed because of the similarities of running the CIPWFULL rogram with or without the P2O5 column.
</commit_message>
<xml_diff>
--- a/_CIPW/CIPW/1_normalized_QAPF_count.xlsx
+++ b/_CIPW/CIPW/1_normalized_QAPF_count.xlsx
@@ -380,7 +380,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>3298</v>
+        <v>3256</v>
       </c>
     </row>
     <row r="3">
@@ -390,7 +390,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>673</v>
+        <v>678</v>
       </c>
     </row>
     <row r="4">
@@ -401,7 +401,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>341</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5">
@@ -411,7 +411,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>252</v>
+        <v>270</v>
       </c>
     </row>
     <row r="6">
@@ -421,7 +421,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7">
@@ -431,7 +431,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8">
@@ -451,7 +451,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10">
@@ -461,7 +461,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -479,7 +479,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>quartz syenite</t>
+          <t>diorite gabbro anorthosite</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -489,7 +489,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>diorite gabbro anorthosite</t>
+          <t>quartz syenite</t>
         </is>
       </c>
       <c r="B13" t="n">

</xml_diff>